<commit_message>
wordcloud + web embedding + packed bubble
</commit_message>
<xml_diff>
--- a/data/top_100_marvel_v2.xlsx
+++ b/data/top_100_marvel_v2.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="257">
   <si>
     <t>page_id</t>
   </si>
@@ -1167,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5753,6 +5753,9 @@
       </c>
       <c r="J82" t="s">
         <v>218</v>
+      </c>
+      <c r="K82" t="s">
+        <v>221</v>
       </c>
       <c r="L82" t="s">
         <v>224</v>

</xml_diff>